<commit_message>
paper and analysis stuff
</commit_message>
<xml_diff>
--- a/analysis/figures/Graphing.xlsx
+++ b/analysis/figures/Graphing.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elizabethmonzingo/Desktop/projects/emcotm/analysis/figures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FBE51420-C025-FC46-8A2F-D69AFB0C8752}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{6E921D92-0CE5-C74B-9E92-86FA7C134AC1}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="17040" xr2:uid="{1D7A5AE5-ABDE-0A4A-8A7C-4DFAE2E95D5A}"/>
+    <workbookView xWindow="380" yWindow="460" windowWidth="34100" windowHeight="17540" xr2:uid="{1D7A5AE5-ABDE-0A4A-8A7C-4DFAE2E95D5A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -216,7 +216,7 @@
               <a:effectLst/>
             </c:spPr>
             <c:txPr>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
                 <a:spAutoFit/>
               </a:bodyPr>
               <a:lstStyle/>
@@ -334,7 +334,7 @@
               <a:effectLst/>
             </c:spPr>
             <c:txPr>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
                 <a:spAutoFit/>
               </a:bodyPr>
               <a:lstStyle/>
@@ -426,8 +426,7 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="444"/>
-        <c:overlap val="-90"/>
+        <c:gapWidth val="119"/>
         <c:axId val="1251611039"/>
         <c:axId val="1251579711"/>
       </c:barChart>
@@ -474,12 +473,9 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="all" spc="120" normalizeH="0" baseline="0">
+              <a:defRPr sz="800" b="0" i="0" u="none" strike="noStrike" kern="1200" cap="none" spc="0" normalizeH="0" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
+                  <a:schemeClr val="tx1"/>
                 </a:solidFill>
                 <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
@@ -521,7 +517,17 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="tr"/>
-      <c:overlay val="0"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.74541882597638665"/>
+          <c:y val="0.12778702163061564"/>
+          <c:w val="0.20098174539883187"/>
+          <c:h val="0.10462830572402357"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="1"/>
       <c:spPr>
         <a:noFill/>
         <a:ln>
@@ -1135,7 +1141,7 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>584200</xdr:colOff>
+      <xdr:colOff>533400</xdr:colOff>
       <xdr:row>27</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
@@ -1464,8 +1470,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38BEFD13-1C8C-694B-B6BF-F41B2AF75010}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C3"/>
+    <sheetView tabSelected="1" topLeftCell="F9" zoomScale="192" workbookViewId="0">
+      <selection activeCell="P16" sqref="P16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>